<commit_message>
Added initial changes in dev branch
</commit_message>
<xml_diff>
--- a/gold_tea_sales.xlsx
+++ b/gold_tea_sales.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,16 @@
           <t>Total Amount</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Payment Status</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Amount Paid</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -530,6 +540,8 @@
       <c r="J2" t="n">
         <v>810</v>
       </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -576,6 +588,8 @@
       <c r="J3" t="n">
         <v>420</v>
       </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -622,6 +636,8 @@
       <c r="J4" t="n">
         <v>60</v>
       </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -668,6 +684,8 @@
       <c r="J5" t="n">
         <v>60</v>
       </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -714,6 +732,8 @@
       <c r="J6" t="n">
         <v>60</v>
       </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -760,6 +780,8 @@
       <c r="J7" t="n">
         <v>60</v>
       </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -806,6 +828,8 @@
       <c r="J8" t="n">
         <v>60</v>
       </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -852,6 +876,8 @@
       <c r="J9" t="n">
         <v>60</v>
       </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -897,6 +923,110 @@
       </c>
       <c r="J10" t="n">
         <v>60</v>
+      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-12-31</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>vairgwadi</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Vinayak</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>GOLD Tea Powder</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>100gm</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>60</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>60</v>
+      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-12-31</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>vairgwadi</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Vinayak</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>GOLD Tea Powder</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>100gm</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>60</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>60</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Half paid</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated features / bug fixes
</commit_message>
<xml_diff>
--- a/gold_tea_sales.xlsx
+++ b/gold_tea_sales.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1029,6 +1029,492 @@
         <v>50</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-12-31</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Harali KH</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>sakshi</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>GOLD Tea Powder</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>100gm</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>60</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="n">
+        <v>60</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Half paid</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-12-31</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>vairgwadi</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Suresh Patil</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>GOLD Tea Powder</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>100gm</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>60</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" t="n">
+        <v>60</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Not paid</t>
+        </is>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2026-01-14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Harali KH</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>sakshi</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>GOLD Tea Powder</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>100gm</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>60</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" t="n">
+        <v>60</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Half paid</t>
+        </is>
+      </c>
+      <c r="L15" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-12-31</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>vairgwadi</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Anil Dhotare</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>GOLD Tea Powder</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>100gm</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>35</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" t="n">
+        <v>35</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-12-31</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>vairgwadi</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>geeta Morti</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>GOLD Tea Powder</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>100gm</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>35</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" t="n">
+        <v>35</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-12-31</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Harali KH</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>sakshi</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>GOLD Tea Powder</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>500gm</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>170</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" t="n">
+        <v>170</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Half paid</t>
+        </is>
+      </c>
+      <c r="L18" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2026-01-02</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Harali BK</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Ramdas Salve</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>GOLD Tea Powder</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>500gm</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>170</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" t="n">
+        <v>170</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Half paid</t>
+        </is>
+      </c>
+      <c r="L19" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2026-01-01</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>vairgwadi</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Hausabai Murkute</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>GOLD Tea Powder</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>100gm</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>35</v>
+      </c>
+      <c r="I20" t="n">
+        <v>2</v>
+      </c>
+      <c r="J20" t="n">
+        <v>70</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2026-01-01</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Harali BK</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Hari Patake</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>GOLD Tea Powder</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>100gm</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>35</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" t="n">
+        <v>35</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>